<commit_message>
SPI with FLASH tests working
Signed-off-by: bigbass1997 <bigbass1997.website@gmail.com>
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -696,7 +696,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1124,13 +1124,13 @@
         <v>40</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1157,13 +1157,13 @@
         <v>41</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added external TAS start button and added LED indicator.
Signed-off-by: bigbass1997 <bigbass1997.website@gmail.com>
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -88,6 +88,12 @@
     <t xml:space="preserve">RB5</t>
   </si>
   <si>
+    <t xml:space="preserve">INT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replay Toggle</t>
+  </si>
+  <si>
     <t xml:space="preserve">PORTC</t>
   </si>
   <si>
@@ -143,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">VDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STAT_LED</t>
   </si>
   <si>
     <t xml:space="preserve">RE2</t>
@@ -562,12 +571,12 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.43"/>
@@ -577,7 +586,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="3.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
   </cols>
@@ -708,11 +717,17 @@
       <c r="H4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="N4" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O4" s="11"/>
     </row>
@@ -722,10 +737,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>4</v>
@@ -735,13 +750,13 @@
         <v>37</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="N5" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O5" s="12"/>
     </row>
@@ -751,10 +766,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>5</v>
@@ -764,13 +779,13 @@
         <v>36</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="N6" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O6" s="13"/>
     </row>
@@ -780,10 +795,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="9" t="n">
         <v>6</v>
@@ -793,13 +808,13 @@
         <v>35</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="N7" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O7" s="7"/>
     </row>
@@ -808,7 +823,7 @@
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" s="9" t="n">
         <v>7</v>
@@ -818,7 +833,7 @@
         <v>34</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -829,7 +844,7 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E9" s="13" t="n">
         <v>8</v>
@@ -839,7 +854,7 @@
         <v>33</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -850,7 +865,7 @@
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E10" s="13" t="n">
         <v>9</v>
@@ -860,7 +875,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -868,10 +883,14 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E11" s="13" t="n">
         <v>10</v>
@@ -881,7 +900,7 @@
         <v>31</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -892,7 +911,7 @@
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" s="14" t="n">
         <v>11</v>
@@ -902,7 +921,7 @@
         <v>30</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -913,7 +932,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E13" s="15" t="n">
         <v>12</v>
@@ -923,7 +942,7 @@
         <v>29</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
@@ -934,7 +953,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E14" s="9" t="n">
         <v>13</v>
@@ -944,7 +963,7 @@
         <v>28</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
@@ -955,7 +974,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E15" s="9" t="n">
         <v>14</v>
@@ -965,7 +984,7 @@
         <v>27</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -976,7 +995,7 @@
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E16" s="11" t="n">
         <v>15</v>
@@ -986,7 +1005,7 @@
         <v>26</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -997,7 +1016,7 @@
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E17" s="11" t="n">
         <v>16</v>
@@ -1007,30 +1026,30 @@
         <v>25</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E18" s="11" t="n">
         <v>17</v>
@@ -1040,30 +1059,30 @@
         <v>24</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E19" s="11" t="n">
         <v>18</v>
@@ -1073,30 +1092,30 @@
         <v>23</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E20" s="12" t="n">
         <v>19</v>
@@ -1106,7 +1125,7 @@
         <v>22</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -1118,10 +1137,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E21" s="12" t="n">
         <v>20</v>
@@ -1131,7 +1150,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>

</xml_diff>

<commit_message>
Added automatic NES reset capability
Signed-off-by: bigbass1997 <bigbass1997.website@gmail.com>
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">RB0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CON_RESET</t>
   </si>
   <si>
     <t xml:space="preserve">RE1</t>
@@ -571,7 +574,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,10 +865,14 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="D10" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E10" s="13" t="n">
         <v>9</v>
@@ -875,7 +882,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -887,10 +894,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" s="13" t="n">
         <v>10</v>
@@ -900,7 +907,7 @@
         <v>31</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -911,7 +918,7 @@
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="14" t="n">
         <v>11</v>
@@ -921,7 +928,7 @@
         <v>30</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -932,7 +939,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="15" t="n">
         <v>12</v>
@@ -942,7 +949,7 @@
         <v>29</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
@@ -953,7 +960,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="9" t="n">
         <v>13</v>
@@ -963,7 +970,7 @@
         <v>28</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
@@ -974,7 +981,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" s="9" t="n">
         <v>14</v>
@@ -984,7 +991,7 @@
         <v>27</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -995,7 +1002,7 @@
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E16" s="11" t="n">
         <v>15</v>
@@ -1005,7 +1012,7 @@
         <v>26</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1016,7 +1023,7 @@
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" s="11" t="n">
         <v>16</v>
@@ -1026,30 +1033,30 @@
         <v>25</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" s="11" t="n">
         <v>17</v>
@@ -1059,30 +1066,30 @@
         <v>24</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" s="11" t="n">
         <v>18</v>
@@ -1092,30 +1099,30 @@
         <v>23</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="12" t="n">
         <v>19</v>
@@ -1125,7 +1132,7 @@
         <v>22</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -1137,10 +1144,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E21" s="12" t="n">
         <v>20</v>
@@ -1150,7 +1157,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>

</xml_diff>

<commit_message>
Updated schematic and prototype PCB design.
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Primary MCU" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MCU-Play" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MCU-Viz" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="90">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -49,7 +50,7 @@
     <t xml:space="preserve">RE3</t>
   </si>
   <si>
-    <t xml:space="preserve">PIC18LF57K42</t>
+    <t xml:space="preserve">PIC18F57K42</t>
   </si>
   <si>
     <t xml:space="preserve">RB7</t>
@@ -254,6 +255,42 @@
   </si>
   <si>
     <t xml:space="preserve">RD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIC18F27K42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART--&gt;MCU_PLAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STROBE0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART&lt;--MCU_PLAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STROBE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STROBE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STROBE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB--&gt;UART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB&lt;--UART</t>
   </si>
 </sst>
 </file>
@@ -573,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1176,4 +1213,583 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="3.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="N2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="n">
+        <v>27</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="N3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="10" t="n">
+        <v>26</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10" t="n">
+        <v>23</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10" t="n">
+        <v>22</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10" t="n">
+        <v>21</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="15" t="n">
+        <v>19</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F2:F15"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Major overhaul to visual input display feature.
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="92">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -50,7 +50,7 @@
     <t xml:space="preserve">RE3</t>
   </si>
   <si>
-    <t xml:space="preserve">PIC18F57K42</t>
+    <t xml:space="preserve">PIC18F47K42</t>
   </si>
   <si>
     <t xml:space="preserve">RB7</t>
@@ -188,6 +188,18 @@
     <t xml:space="preserve">RC7</t>
   </si>
   <si>
+    <t xml:space="preserve">FLASH_CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flash Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write to Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART_HOST</t>
+  </si>
+  <si>
     <t xml:space="preserve">RC1</t>
   </si>
   <si>
@@ -234,12 +246,6 @@
   </si>
   <si>
     <t xml:space="preserve">CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS/CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPI1SS</t>
   </si>
   <si>
     <t xml:space="preserve">RD0</t>
@@ -611,7 +617,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1051,16 +1057,28 @@
       <c r="H16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="I16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E17" s="11" t="n">
         <v>16</v>
@@ -1070,30 +1088,30 @@
         <v>25</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E18" s="11" t="n">
         <v>17</v>
@@ -1103,30 +1121,30 @@
         <v>24</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E19" s="11" t="n">
         <v>18</v>
@@ -1136,30 +1154,24 @@
         <v>23</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>72</v>
-      </c>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" s="12" t="n">
         <v>19</v>
@@ -1169,7 +1181,7 @@
         <v>22</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -1181,10 +1193,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E21" s="12" t="n">
         <v>20</v>
@@ -1194,7 +1206,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -1223,7 +1235,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1295,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>28</v>
@@ -1362,13 +1374,13 @@
         <v>21</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>24</v>
@@ -1377,9 +1389,11 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>26</v>
@@ -1395,13 +1409,13 @@
         <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>36</v>
@@ -1410,9 +1424,11 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>30</v>
@@ -1427,17 +1443,25 @@
       <c r="H6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="N6" s="0"/>
       <c r="O6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>34</v>
@@ -1460,9 +1484,11 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C8" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>37</v>
@@ -1546,13 +1572,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>53</v>
@@ -1573,16 +1599,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E13" s="11" t="n">
         <v>12</v>
@@ -1592,7 +1618,7 @@
         <v>17</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1600,16 +1626,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E14" s="11" t="n">
         <v>13</v>
@@ -1619,7 +1645,7 @@
         <v>16</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1627,16 +1653,16 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E15" s="11" t="n">
         <v>14</v>
@@ -1646,7 +1672,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>

</xml_diff>

<commit_message>
Added NES vizboard input display. Reorganized hardware directories. Changed license to the more suitable CERN OHL-W
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -9,7 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="MCU-Play" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="MCU-Viz" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MCU-Play_Redesign" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MCU-Viz" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="105">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -261,6 +262,153 @@
   </si>
   <si>
     <t xml:space="preserve">RD2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">GEN/A2600/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NES_LATCH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">GEN/A2600/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NES_CLK1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">GEN/A2600/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NES_DATA1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">GEN/A2600/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NES_CLK2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">GEN/A2600/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NES_DATA2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN/A2600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N64_DATA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N64_DATA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N64_DATA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N64_DATA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB/GEN/A2600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">/GEN/A2600</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">PIC18F27K42</t>
@@ -306,7 +454,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -374,6 +522,12 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -472,7 +626,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -534,6 +688,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,7 +779,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -864,7 +1026,7 @@
       </c>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -956,7 +1118,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -977,7 +1139,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -998,7 +1160,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1019,7 +1181,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1232,10 +1394,679 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="3.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="N2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="n">
+        <v>39</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="N3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="10" t="n">
+        <v>38</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="N5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10" t="n">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10" t="n">
+        <v>34</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="12" t="n">
+        <v>29</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="12" t="n">
+        <v>27</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="11" t="n">
+        <v>26</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="12" t="n">
+        <v>19</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="12" t="n">
+        <v>22</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="12" t="n">
+        <v>21</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F2:F21"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1307,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>28</v>
@@ -1374,13 +2205,13 @@
         <v>21</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>24</v>
@@ -1393,7 +2224,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>26</v>
@@ -1409,13 +2240,13 @@
         <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>36</v>
@@ -1428,7 +2259,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>30</v>
@@ -1461,7 +2292,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>34</v>
@@ -1488,7 +2319,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>37</v>
@@ -1572,7 +2403,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>6</v>
@@ -1626,7 +2457,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>13</v>
@@ -1653,7 +2484,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Revised PCB design again.
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="109">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -264,109 +264,19 @@
     <t xml:space="preserve">RD2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">GEN/A2600/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NES_LATCH</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">GEN/A2600/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NES_CLK1 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">GEN/A2600/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NES_DATA1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">GEN/A2600/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NES_CLK2 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">GEN/A2600/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NES_DATA2</t>
-    </r>
+    <t xml:space="preserve">GEN/A2600/NES_LATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN/A2600/NES_CLK1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN/A2600/NES_DATA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN/A2600/NES_CLK2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN/A2600/NES_DATA2</t>
   </si>
   <si>
     <t xml:space="preserve">GEN/A2600</t>
@@ -378,6 +288,12 @@
     <t xml:space="preserve">N64_DATA3</t>
   </si>
   <si>
+    <t xml:space="preserve">Alternative CLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALT_CLK</t>
+  </si>
+  <si>
     <t xml:space="preserve">N64_DATA2</t>
   </si>
   <si>
@@ -390,25 +306,13 @@
     <t xml:space="preserve">GB</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">GB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">/GEN/A2600</t>
-    </r>
+    <t xml:space="preserve">Reset Console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OEOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odd/Even Field</t>
   </si>
   <si>
     <t xml:space="preserve">PIC18F27K42</t>
@@ -454,7 +358,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -522,12 +426,6 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -626,7 +524,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -688,14 +586,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1397,12 +1287,12 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.43"/>
@@ -1412,7 +1302,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="3.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
   </cols>
@@ -1494,7 +1384,7 @@
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="9" t="s">
         <v>80</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1527,7 +1417,7 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="9" t="s">
         <v>81</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1562,7 +1452,7 @@
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1591,7 +1481,7 @@
       <c r="B6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="9" t="s">
         <v>83</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -1626,7 +1516,7 @@
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="9" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -1661,7 +1551,7 @@
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1825,9 +1715,15 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="D14" s="9" t="s">
         <v>49</v>
       </c>
@@ -1841,8 +1737,8 @@
       <c r="H14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>88</v>
+      <c r="I14" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>1</v>
@@ -1854,7 +1750,7 @@
       <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -1870,8 +1766,8 @@
       <c r="H15" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>89</v>
+      <c r="I15" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>1</v>
@@ -1884,7 +1780,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>53</v>
@@ -1900,7 +1796,7 @@
         <v>54</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>6</v>
@@ -1997,7 +1893,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="17"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
         <v>75</v>
       </c>
@@ -2011,14 +1907,20 @@
       <c r="H20" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="17"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="D21" s="12" t="s">
         <v>78</v>
       </c>
@@ -2032,9 +1934,15 @@
       <c r="H21" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="17"/>
+      <c r="I21" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2065,7 +1973,7 @@
   </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2138,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>28</v>
@@ -2205,13 +2113,13 @@
         <v>21</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>24</v>
@@ -2224,7 +2132,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>26</v>
@@ -2240,13 +2148,13 @@
         <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>36</v>
@@ -2259,7 +2167,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>30</v>
@@ -2292,7 +2200,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>34</v>
@@ -2319,7 +2227,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>37</v>
@@ -2403,7 +2311,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>6</v>
@@ -2457,7 +2365,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>13</v>
@@ -2484,7 +2392,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Partially working. SPI to FLASH has severe issues on PCB
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MCU-Play" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MCU-Play_Redesign" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="MCU-Viz" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="MCU-Play_Redesign_Fixed" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="MCU-Viz" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="110">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -313,6 +314,9 @@
   </si>
   <si>
     <t xml:space="preserve">Odd/Even Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI1SDOI</t>
   </si>
   <si>
     <t xml:space="preserve">PIC18F27K42</t>
@@ -1286,8 +1290,8 @@
   </sheetPr>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1379,7 +1383,7 @@
       </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -1447,7 +1451,7 @@
       </c>
       <c r="O4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -1468,9 +1472,15 @@
       <c r="H5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="N5" s="12" t="s">
         <v>28</v>
       </c>
@@ -1971,10 +1981,691 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="3.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="N2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="n">
+        <v>39</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="N3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="10" t="n">
+        <v>38</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10" t="n">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10" t="n">
+        <v>34</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="12" t="n">
+        <v>29</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="12" t="n">
+        <v>27</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="11" t="n">
+        <v>26</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="12" t="n">
+        <v>19</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="12" t="n">
+        <v>22</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="12" t="n">
+        <v>21</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F2:F21"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2046,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>28</v>
@@ -2113,13 +2804,13 @@
         <v>21</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>24</v>
@@ -2132,7 +2823,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>26</v>
@@ -2148,13 +2839,13 @@
         <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>36</v>
@@ -2167,7 +2858,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>30</v>
@@ -2200,7 +2891,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>34</v>
@@ -2227,7 +2918,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>37</v>
@@ -2311,7 +3002,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>6</v>
@@ -2365,7 +3056,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>13</v>
@@ -2392,7 +3083,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
New firmware confirmed to be able to program FLASH and verified using mass dump.
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MCU-Play" sheetId="1" state="visible" r:id="rId2"/>
@@ -1290,7 +1290,7 @@
   </sheetPr>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1983,8 +1983,8 @@
   </sheetPr>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2664,7 +2664,7 @@
   </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atari 2600 and beginner Genesis work; reorganized firmware.
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="MCU-Play" sheetId="1" state="visible" r:id="rId2"/>
@@ -59,6 +59,9 @@
     <t xml:space="preserve">ICSPDAT</t>
   </si>
   <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
     <t xml:space="preserve">PORTA</t>
   </si>
   <si>
@@ -105,9 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">U1RX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
   </si>
   <si>
     <t xml:space="preserve">UART1 RX</t>
@@ -640,8 +640,8 @@
   </sheetPr>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -725,11 +725,11 @@
         <v>11</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K2" s="7"/>
       <c r="N2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O2" s="9"/>
     </row>
@@ -739,10 +739,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="9" t="n">
         <v>2</v>
@@ -752,17 +752,17 @@
         <v>39</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K3" s="7"/>
       <c r="N3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O3" s="10"/>
     </row>
@@ -772,10 +772,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9" t="n">
         <v>3</v>
@@ -785,19 +785,19 @@
         <v>38</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4" s="11"/>
     </row>
@@ -807,10 +807,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>4</v>
@@ -820,13 +820,13 @@
         <v>37</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>29</v>
@@ -958,7 +958,7 @@
         <v>50</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>51</v>
@@ -1067,7 +1067,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>63</v>
@@ -1286,7 +1286,7 @@
         <v>86</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K21" s="12" t="s">
         <v>87</v>
@@ -1325,8 +1325,8 @@
   </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="K2" s="7"/>
       <c r="N2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O2" s="9"/>
     </row>
@@ -1423,7 +1423,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="9" t="n">
         <v>2</v>
@@ -1433,17 +1433,17 @@
         <v>27</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="7"/>
       <c r="N3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O3" s="10"/>
     </row>
@@ -1452,7 +1452,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9" t="n">
         <v>3</v>
@@ -1462,19 +1462,19 @@
         <v>26</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>89</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>90</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4" s="11"/>
     </row>
@@ -1487,7 +1487,7 @@
         <v>91</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>4</v>
@@ -1497,7 +1497,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>92</v>
@@ -1538,7 +1538,7 @@
         <v>55</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>54</v>
@@ -1720,10 +1720,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>76</v>
@@ -1750,7 +1750,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>78</v>

</xml_diff>